<commit_message>
add android sdk url.
</commit_message>
<xml_diff>
--- a/IT_space.xlsx
+++ b/IT_space.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="地图" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="322">
   <si>
     <t>服务器</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1234,23 +1234,84 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>天行者</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>四川斯盖克科技有限公司</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>skyker  -   Skywalker</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>skk</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>斯盖克</t>
+    <t>移动互联网</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>物联网</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>人工智能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>互联网金融</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>watchOS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cocoa(OS X)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cocoa Touch(iOS)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Betago</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>贝塔狗</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>四川贝塔狗科技有限公司</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>向google的alghago团队致敬；</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>beta：永远的测试版，意味创新；</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>go: 狗，忠诚，人类友好；</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>www.betago.com.cn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>注册资本10万元</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>科学研究</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NumPy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.numpy.org/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.androiddevtools.cn/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1460,7 +1521,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1535,6 +1596,12 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1837,14 +1904,14 @@
   <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="17.25" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.25" style="4" customWidth="1"/>
     <col min="4" max="4" width="11.625" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.625" style="4" customWidth="1"/>
     <col min="6" max="6" width="15" style="4" bestFit="1" customWidth="1"/>
@@ -2577,6 +2644,17 @@
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
     </row>
+    <row r="41" spans="1:9">
+      <c r="B41" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>306</v>
+      </c>
+    </row>
     <row r="42" spans="1:9" ht="12.75">
       <c r="B42" s="19"/>
     </row>
@@ -2589,11 +2667,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G101"/>
+  <dimension ref="A1:G102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A102" sqref="A102"/>
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B107" sqref="B107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2609,10 +2687,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="18" customFormat="1" ht="14.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="25"/>
+      <c r="B1" s="27"/>
       <c r="C1" s="18" t="s">
         <v>270</v>
       </c>
@@ -3708,6 +3786,20 @@
       </c>
       <c r="D101" t="s">
         <v>278</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102" s="7" t="s">
+        <v>317</v>
+      </c>
+      <c r="B102" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="C102" s="7" t="s">
+        <v>319</v>
+      </c>
+      <c r="D102" t="s">
+        <v>320</v>
       </c>
     </row>
   </sheetData>
@@ -3726,10 +3818,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3819,10 +3911,18 @@
         <v>188</v>
       </c>
     </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="26" t="s">
+        <v>321</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A17" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3831,7 +3931,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3953,42 +4053,78 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="27.375" customWidth="1"/>
+    <col min="1" max="1" width="30.625" customWidth="1"/>
     <col min="5" max="5" width="25" customWidth="1"/>
+    <col min="7" max="7" width="16.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7">
+      <c r="G2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>309</v>
+      </c>
+      <c r="B3" t="s">
+        <v>310</v>
+      </c>
+      <c r="E3" t="s">
+        <v>311</v>
+      </c>
+      <c r="G3" s="25" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>312</v>
+      </c>
+      <c r="E4" t="s">
+        <v>316</v>
+      </c>
+      <c r="G4" t="s">
         <v>304</v>
       </c>
-      <c r="B2" t="s">
-        <v>302</v>
-      </c>
-      <c r="C2" t="s">
-        <v>306</v>
-      </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>313</v>
+      </c>
+      <c r="G5" s="25" t="s">
         <v>305</v>
       </c>
-      <c r="E2" t="s">
-        <v>303</v>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="26" t="s">
+        <v>315</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A8" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>